<commit_message>
Integrate the Game creation process
</commit_message>
<xml_diff>
--- a/Documents/BusinessSimulation.xlsx
+++ b/Documents/BusinessSimulation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19095" windowHeight="8670"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19095" windowHeight="8670" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="R&amp;D" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
   <si>
     <t>Able</t>
   </si>
@@ -229,7 +229,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$$-409]#,##0"/>
     <numFmt numFmtId="167" formatCode="&quot;Rs.&quot;\ #,##0.00"/>
-    <numFmt numFmtId="169" formatCode="[$$-409]#,##0.00_ ;\-[$$-409]#,##0.00\ "/>
+    <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00_ ;\-[$$-409]#,##0.00\ "/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -275,7 +275,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -574,8 +574,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -922,7 +922,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1094,10 +1094,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1106,364 +1106,680 @@
     <col min="13" max="13" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:17" hidden="1">
       <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" hidden="1">
+      <c r="A2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" hidden="1">
+      <c r="A3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="38.25">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1188</v>
+      </c>
+      <c r="D5" s="5">
+        <v>11.59</v>
+      </c>
+      <c r="E5" s="5">
+        <f>IF(O5&lt;=100%,HR!$A$23/H5, (100%*HR!$A$23/H5+((O5-100%)*1.5*HR!$A$23/H5)))</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5" s="5">
+        <f>(I5-H5)*$B$1</f>
+        <v>700</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1800</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="7">
+        <f>L5*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <f>C5/H5*$B$3</f>
+        <v>196.02</v>
+      </c>
+      <c r="O5" s="10">
+        <f>$N$10/$P$5</f>
+        <v>1.16974</v>
+      </c>
+      <c r="P5" s="6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1802</v>
+      </c>
+      <c r="D6" s="5">
+        <v>7.81</v>
+      </c>
+      <c r="E6" s="5">
+        <f>IF(O6&lt;=100%,HR!$A$23/H6, (100%*HR!$A$23/H6+((O6-100%)*1.5*HR!$A$23/H6)))</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6" s="5">
+        <f>(I6-H6)*$B$1</f>
+        <v>700</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1400</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="7">
+        <f>L6*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <f>C6/H6*$B$3</f>
+        <v>237.864</v>
+      </c>
+      <c r="O6" s="10">
+        <f>$N$10/$P$5</f>
+        <v>1.16974</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>406</v>
+      </c>
+      <c r="D7" s="5">
+        <v>15.98</v>
+      </c>
+      <c r="E7" s="5">
+        <f>IF(O7&lt;=100%,HR!$A$23/H7, (100%*HR!$A$23/H7+((O7-100%)*1.5*HR!$A$23/H7)))</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7" s="5">
+        <f>(I7-H7)*$B$1</f>
+        <v>700</v>
+      </c>
+      <c r="K7">
+        <v>900</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="7">
+        <f>L7*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <f>C7/H7*$B$3</f>
+        <v>89.320000000000007</v>
+      </c>
+      <c r="O7" s="10">
+        <f>$N$10/$P$5</f>
+        <v>1.16974</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>436</v>
+      </c>
+      <c r="D8" s="5">
+        <v>15.87</v>
+      </c>
+      <c r="E8" s="5">
+        <f>IF(O8&lt;=100%,HR!$A$23/H8, (100%*HR!$A$23/H8+((O8-100%)*1.5*HR!$A$23/H8)))</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8" s="5">
+        <f>(I8-H8)*$B$1</f>
+        <v>700</v>
+      </c>
+      <c r="K8">
+        <v>600</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="7">
+        <f>L8*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <f>C8/H8*$B$3</f>
+        <v>95.920000000000016</v>
+      </c>
+      <c r="O8" s="10">
+        <f>$N$10/$P$5</f>
+        <v>1.16974</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>376</v>
+      </c>
+      <c r="D9" s="5">
+        <v>13.62</v>
+      </c>
+      <c r="E9" s="5">
+        <f>IF(O9&lt;=100%,HR!$A$23/H9, (100%*HR!$A$23/H9+((O9-100%)*1.5*HR!$A$23/H9)))</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9" s="5">
+        <f>(I9-H9)*$B$1</f>
+        <v>700</v>
+      </c>
+      <c r="K9">
+        <v>600</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="7">
+        <f>L9*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <f>C9/H9*$B$3</f>
+        <v>82.72</v>
+      </c>
+      <c r="O9" s="10">
+        <f>$N$10/$P$5</f>
+        <v>1.16974</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="3" t="s">
+      <c r="N10" s="2">
+        <f>SUM(N5:N9)</f>
+        <v>701.84400000000005</v>
+      </c>
+      <c r="O10" s="12"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="25.5">
-      <c r="A3" s="3" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="25.5">
+      <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B3">
+      <c r="B14">
         <v>1188</v>
       </c>
-      <c r="C3">
+      <c r="C14">
         <v>1802</v>
       </c>
-      <c r="D3">
+      <c r="D14">
         <v>406</v>
       </c>
-      <c r="E3">
+      <c r="E14">
         <v>436</v>
       </c>
-      <c r="F3">
+      <c r="F14">
         <v>376</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="3" t="s">
+    <row r="15" spans="1:17">
+      <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B15" s="5">
         <v>11.59</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C15" s="5">
         <v>7.81</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D15" s="5">
         <v>15.98</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E15" s="5">
         <v>15.87</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F15" s="5">
         <v>13.62</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="3" t="s">
+    <row r="16" spans="1:17">
+      <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="5">
-        <f>IF(B15&lt;=100%,HR!$B$1/B8, (100%*HR!$B$1/B8+((B15-100%)*1.5*HR!$B$1/B8)))</f>
+      <c r="B16" s="5">
+        <f>IF(B26&lt;=100%,HR!$B$1/B19, (100%*HR!$B$1/B19+((B26-100%)*1.5*HR!$B$1/B19)))</f>
         <v>8.7822700000000005</v>
       </c>
-      <c r="C5" s="5">
-        <f>IF(C15&lt;=100%,HR!$B$1/C8, (100%*HR!$B$1/C8+((C15-100%)*1.5*HR!$B$1/C8)))</f>
+      <c r="C16" s="5">
+        <f>IF(C26&lt;=100%,HR!$B$1/C19, (100%*HR!$B$1/C19+((C26-100%)*1.5*HR!$B$1/C19)))</f>
         <v>7.0258159999999998</v>
       </c>
-      <c r="D5" s="5">
-        <f>IF(D15&lt;=100%,HR!$B$1/D8, (100%*HR!$B$1/D8+((D15-100%)*1.5*HR!$B$1/D8)))</f>
+      <c r="D16" s="5">
+        <f>IF(D26&lt;=100%,HR!$B$1/D19, (100%*HR!$B$1/D19+((D26-100%)*1.5*HR!$B$1/D19)))</f>
         <v>11.709693333333334</v>
       </c>
-      <c r="E5" s="5">
-        <f>IF(E15&lt;=100%,HR!$B$1/E8, (100%*HR!$B$1/E8+((E15-100%)*1.5*HR!$B$1/E8)))</f>
+      <c r="E16" s="5">
+        <f>IF(E26&lt;=100%,HR!$B$1/E19, (100%*HR!$B$1/E19+((E26-100%)*1.5*HR!$B$1/E19)))</f>
         <v>11.709693333333334</v>
       </c>
-      <c r="F5" s="5">
-        <f>IF(F15&lt;=100%,HR!$B$1/F8, (100%*HR!$B$1/F8+((F15-100%)*1.5*HR!$B$1/F8)))</f>
+      <c r="F16" s="5">
+        <f>IF(F26&lt;=100%,HR!$B$1/F19, (100%*HR!$B$1/F19+((F26-100%)*1.5*HR!$B$1/F19)))</f>
         <v>11.709693333333334</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
+    <row r="17" spans="1:7">
+      <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B17" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C17" s="1">
         <v>0.27</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D17" s="1">
         <v>0.33</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E17" s="1">
         <v>0.23</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F17" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="25.5">
-      <c r="A7" s="3" t="s">
+    <row r="18" spans="1:7" ht="25.5">
+      <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
         <v>0.3</v>
       </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="3" t="s">
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B8">
+      <c r="B19">
         <v>4</v>
       </c>
-      <c r="C8">
+      <c r="C19">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="D19">
         <v>3</v>
       </c>
-      <c r="E8">
+      <c r="E19">
         <v>3</v>
       </c>
-      <c r="F8">
+      <c r="F19">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="25.5">
-      <c r="A9" s="3" t="s">
+    <row r="20" spans="1:7" ht="25.5">
+      <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B9">
+      <c r="B20">
         <v>5</v>
       </c>
-      <c r="C9">
+      <c r="C20">
         <v>6</v>
       </c>
-      <c r="D9">
+      <c r="D20">
         <v>4</v>
       </c>
-      <c r="E9">
+      <c r="E20">
         <v>4</v>
       </c>
-      <c r="F9">
+      <c r="F20">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
+    <row r="21" spans="1:7">
+      <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="5">
-        <f>(B9-B8)*$B$19</f>
+      <c r="B21" s="5">
+        <f>(B20-B19)*$B$1</f>
         <v>700</v>
       </c>
-      <c r="C10" s="5">
-        <f t="shared" ref="C10:F10" si="0">(C9-C8)*$B$19</f>
+      <c r="C21" s="5">
+        <f t="shared" ref="C21:F21" si="0">(C20-C19)*$B$1</f>
         <v>700</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D21" s="5">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E21" s="5">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F21" s="5">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="25.5">
-      <c r="A11" s="3" t="s">
+    <row r="22" spans="1:7" ht="25.5">
+      <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B22" s="2">
         <v>1800</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C22" s="2">
         <v>1400</v>
       </c>
-      <c r="D11">
+      <c r="D22">
         <v>900</v>
       </c>
-      <c r="E11">
+      <c r="E22">
         <v>600</v>
       </c>
-      <c r="F11">
+      <c r="F22">
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="3" t="s">
+    <row r="23" spans="1:7">
+      <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="7">
-        <f>B12*$B$20</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="7">
-        <f t="shared" ref="C13:F13" si="1">C12*$B$20</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="B24" s="7">
+        <f>B23*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" ref="C24:F24" si="1">C23*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E24" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F24" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="3" t="s">
+    <row r="25" spans="1:7">
+      <c r="A25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="2">
-        <f>B3/B8*$B$21</f>
+      <c r="B25" s="2">
+        <f>B14/B19*$B$3</f>
         <v>196.02</v>
       </c>
-      <c r="C14" s="2">
-        <f t="shared" ref="C14:F14" si="2">C3/C8*$B$21</f>
+      <c r="C25" s="2">
+        <f t="shared" ref="C25:F25" si="2">C14/C19*$B$3</f>
         <v>237.864</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D25" s="2">
         <f t="shared" si="2"/>
         <v>89.320000000000007</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E25" s="2">
         <f t="shared" si="2"/>
         <v>95.920000000000016</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F25" s="2">
         <f t="shared" si="2"/>
         <v>82.72</v>
       </c>
-      <c r="G14" s="2">
-        <f>SUM(B14:F14)</f>
+      <c r="G25" s="2">
+        <f>SUM(B25:F25)</f>
         <v>701.84400000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="3" t="s">
+    <row r="26" spans="1:7">
+      <c r="A26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="10">
-        <f>$G$14/$B$16</f>
+      <c r="B26" s="10">
+        <f>$G$25/$B$27</f>
         <v>1.16974</v>
       </c>
-      <c r="C15" s="10">
-        <f t="shared" ref="C15:F15" si="3">$G$14/$B$16</f>
+      <c r="C26" s="10">
+        <f>$G$25/$B$27</f>
         <v>1.16974</v>
       </c>
-      <c r="D15" s="10">
-        <f t="shared" si="3"/>
+      <c r="D26" s="10">
+        <f>$G$25/$B$27</f>
         <v>1.16974</v>
       </c>
-      <c r="E15" s="10">
-        <f t="shared" si="3"/>
+      <c r="E26" s="10">
+        <f>$G$25/$B$27</f>
         <v>1.16974</v>
       </c>
-      <c r="F15" s="10">
-        <f t="shared" si="3"/>
+      <c r="F26" s="10">
+        <f>$G$25/$B$27</f>
         <v>1.16974</v>
       </c>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="3" t="s">
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B27" s="6">
         <v>600</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+    <row r="28" spans="1:7">
+      <c r="A28" s="3" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" hidden="1">
-      <c r="A19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" hidden="1">
-      <c r="A20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" hidden="1">
-      <c r="A21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21">
-        <v>0.66</v>
       </c>
     </row>
   </sheetData>
@@ -1611,23 +1927,23 @@
         <v>20</v>
       </c>
       <c r="B4" s="5">
-        <f>Production!B3*Production!B5</f>
+        <f>Production!B14*Production!B16</f>
         <v>10433.33676</v>
       </c>
       <c r="C4" s="5">
-        <f>Production!C3*Production!C5</f>
+        <f>Production!C14*Production!C16</f>
         <v>12660.520431999999</v>
       </c>
       <c r="D4" s="5">
-        <f>Production!D3*Production!D5</f>
+        <f>Production!D14*Production!D16</f>
         <v>4754.1354933333332</v>
       </c>
       <c r="E4" s="5">
-        <f>Production!E3*Production!E5</f>
+        <f>Production!E14*Production!E16</f>
         <v>5105.4262933333339</v>
       </c>
       <c r="F4" s="5">
-        <f>Production!F3*Production!F5</f>
+        <f>Production!F14*Production!F16</f>
         <v>4402.8446933333335</v>
       </c>
       <c r="G4" s="5">
@@ -1640,23 +1956,23 @@
         <v>19</v>
       </c>
       <c r="B5" s="5">
-        <f>Production!B4*Production!B3</f>
+        <f>Production!B15*Production!B14</f>
         <v>13768.92</v>
       </c>
       <c r="C5" s="5">
-        <f>Production!C4*Production!C3</f>
+        <f>Production!C15*Production!C14</f>
         <v>14073.619999999999</v>
       </c>
       <c r="D5" s="5">
-        <f>Production!D4*Production!D3</f>
+        <f>Production!D15*Production!D14</f>
         <v>6487.88</v>
       </c>
       <c r="E5" s="5">
-        <f>Production!E4*Production!E3</f>
+        <f>Production!E15*Production!E14</f>
         <v>6919.32</v>
       </c>
       <c r="F5" s="5">
-        <f>Production!F4*Production!F3</f>
+        <f>Production!F15*Production!F14</f>
         <v>5121.12</v>
       </c>
       <c r="G5" s="5">
@@ -1669,23 +1985,23 @@
         <v>30</v>
       </c>
       <c r="B6" s="5">
-        <f>Production!B10</f>
+        <f>Production!B21</f>
         <v>700</v>
       </c>
       <c r="C6" s="5">
-        <f>Production!C10</f>
+        <f>Production!C21</f>
         <v>700</v>
       </c>
       <c r="D6" s="5">
-        <f>Production!D10</f>
+        <f>Production!D21</f>
         <v>700</v>
       </c>
       <c r="E6" s="5">
-        <f>Production!E10</f>
+        <f>Production!E21</f>
         <v>700</v>
       </c>
       <c r="F6" s="5">
-        <f>Production!F10</f>
+        <f>Production!F21</f>
         <v>700</v>
       </c>
       <c r="G6" s="5">
@@ -1698,23 +2014,23 @@
         <v>42</v>
       </c>
       <c r="B7" s="5">
-        <f>Production!B13</f>
+        <f>Production!B24</f>
         <v>0</v>
       </c>
       <c r="C7" s="5">
-        <f>Production!C13</f>
+        <f>Production!C24</f>
         <v>0</v>
       </c>
       <c r="D7" s="5">
-        <f>Production!D13</f>
+        <f>Production!D24</f>
         <v>0</v>
       </c>
       <c r="E7" s="5">
-        <f>Production!E13</f>
+        <f>Production!E24</f>
         <v>0</v>
       </c>
       <c r="F7" s="5">
-        <f>Production!F13</f>
+        <f>Production!F24</f>
         <v>0</v>
       </c>
       <c r="G7" s="5">

</xml_diff>

<commit_message>
Uploaded to the server
</commit_message>
<xml_diff>
--- a/Documents/BusinessSimulation.xlsx
+++ b/Documents/BusinessSimulation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
   <si>
     <t>Able</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t xml:space="preserve">Reliability Factor </t>
+  </si>
+  <si>
+    <t>SegmentType</t>
+  </si>
+  <si>
+    <t>Perf</t>
   </si>
 </sst>
 </file>
@@ -1094,10 +1100,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1106,7 +1112,7 @@
     <col min="13" max="13" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" hidden="1">
+    <row r="1" spans="1:18" ht="6" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
@@ -1114,7 +1120,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1">
+    <row r="2" spans="1:18" ht="22.5" hidden="1" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -1122,7 +1128,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1">
+    <row r="3" spans="1:18" ht="31.5" hidden="1" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>47</v>
       </c>
@@ -1130,323 +1136,341 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="38.25">
+    <row r="4" spans="1:18" ht="38.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" t="s">
+        <v>1</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>1188</v>
       </c>
-      <c r="D5" s="5">
+      <c r="E5" s="5">
         <v>11.59</v>
       </c>
-      <c r="E5" s="5">
-        <f>IF(O5&lt;=100%,HR!$A$23/H5, (100%*HR!$A$23/H5+((O5-100%)*1.5*HR!$A$23/H5)))</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
+        <f>IF(P5&lt;=100%,HR!$B$1/I5, (100%*HR!$B$1/I5+((P5-100%)*1.5*HR!$B$1/I5)))</f>
+        <v>8.7822700000000005</v>
+      </c>
+      <c r="G5" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5">
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>4</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>5</v>
       </c>
-      <c r="J5" s="5">
-        <f>(I5-H5)*$B$1</f>
+      <c r="K5" s="5">
+        <f>(J5-I5)*$B$1</f>
         <v>700</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>1800</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="7">
-        <f>L5*$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <f>C5/H5*$B$3</f>
+      <c r="M5" s="1"/>
+      <c r="N5" s="7">
+        <f>M5*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <f>D5/I5*$B$3</f>
         <v>196.02</v>
       </c>
-      <c r="O5" s="10">
-        <f>$N$10/$P$5</f>
+      <c r="P5" s="10">
+        <f>$N$10/$Q$5</f>
         <v>1.16974</v>
       </c>
-      <c r="P5" s="6">
+      <c r="Q5" s="6">
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>0</v>
+      <c r="B6" t="s">
+        <v>3</v>
       </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>1802</v>
       </c>
-      <c r="D6" s="5">
+      <c r="E6" s="5">
         <v>7.81</v>
       </c>
-      <c r="E6" s="5">
-        <f>IF(O6&lt;=100%,HR!$A$23/H6, (100%*HR!$A$23/H6+((O6-100%)*1.5*HR!$A$23/H6)))</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="F6" s="5">
+        <f>IF(P6&lt;=100%,HR!$B$1/I6, (100%*HR!$B$1/I6+((P6-100%)*1.5*HR!$B$1/I6)))</f>
+        <v>7.0258159999999998</v>
+      </c>
+      <c r="G6" s="1">
         <v>0.27</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>0.3</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>5</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>6</v>
       </c>
-      <c r="J6" s="5">
-        <f>(I6-H6)*$B$1</f>
+      <c r="K6" s="5">
+        <f>(J6-I6)*$B$1</f>
         <v>700</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>1400</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="7">
-        <f>L6*$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <f>C6/H6*$B$3</f>
+      <c r="M6" s="1"/>
+      <c r="N6" s="7">
+        <f>M6*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <f>D6/I6*$B$3</f>
         <v>237.864</v>
       </c>
-      <c r="O6" s="10">
-        <f>$N$10/$P$5</f>
+      <c r="P6" s="10">
+        <f>$N$10/$Q$5</f>
         <v>1.16974</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>0</v>
+      <c r="B7" t="s">
+        <v>5</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>406</v>
       </c>
-      <c r="D7" s="5">
+      <c r="E7" s="5">
         <v>15.98</v>
       </c>
-      <c r="E7" s="5">
-        <f>IF(O7&lt;=100%,HR!$A$23/H7, (100%*HR!$A$23/H7+((O7-100%)*1.5*HR!$A$23/H7)))</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="F7" s="5">
+        <f>IF(P7&lt;=100%,HR!$B$1/I7, (100%*HR!$B$1/I7+((P7-100%)*1.5*HR!$B$1/I7)))</f>
+        <v>11.709693333333334</v>
+      </c>
+      <c r="G7" s="1">
         <v>0.33</v>
       </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7">
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>3</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>4</v>
       </c>
-      <c r="J7" s="5">
-        <f>(I7-H7)*$B$1</f>
+      <c r="K7" s="5">
+        <f>(J7-I7)*$B$1</f>
         <v>700</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>900</v>
       </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="7">
-        <f>L7*$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="2">
-        <f>C7/H7*$B$3</f>
+      <c r="M7" s="1"/>
+      <c r="N7" s="7">
+        <f>M7*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <f>D7/I7*$B$3</f>
         <v>89.320000000000007</v>
       </c>
-      <c r="O7" s="10">
-        <f>$N$10/$P$5</f>
+      <c r="P7" s="10">
+        <f>$N$10/$Q$5</f>
         <v>1.16974</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" t="s">
+        <v>66</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>436</v>
       </c>
-      <c r="D8" s="5">
+      <c r="E8" s="5">
         <v>15.87</v>
       </c>
-      <c r="E8" s="5">
-        <f>IF(O8&lt;=100%,HR!$A$23/H8, (100%*HR!$A$23/H8+((O8-100%)*1.5*HR!$A$23/H8)))</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="F8" s="5">
+        <f>IF(P8&lt;=100%,HR!$B$1/I8, (100%*HR!$B$1/I8+((P8-100%)*1.5*HR!$B$1/I8)))</f>
+        <v>11.709693333333334</v>
+      </c>
+      <c r="G8" s="1">
         <v>0.23</v>
       </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8">
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>3</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>4</v>
       </c>
-      <c r="J8" s="5">
-        <f>(I8-H8)*$B$1</f>
+      <c r="K8" s="5">
+        <f>(J8-I8)*$B$1</f>
         <v>700</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>600</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="7">
-        <f>L8*$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="2">
-        <f>C8/H8*$B$3</f>
+      <c r="M8" s="1"/>
+      <c r="N8" s="7">
+        <f>M8*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <f>D8/I8*$B$3</f>
         <v>95.920000000000016</v>
       </c>
-      <c r="O8" s="10">
-        <f>$N$10/$P$5</f>
+      <c r="P8" s="10">
+        <f>$N$10/$Q$5</f>
         <v>1.16974</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>0</v>
+      <c r="B9" t="s">
+        <v>9</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>376</v>
       </c>
-      <c r="D9" s="5">
+      <c r="E9" s="5">
         <v>13.62</v>
       </c>
-      <c r="E9" s="5">
-        <f>IF(O9&lt;=100%,HR!$A$23/H9, (100%*HR!$A$23/H9+((O9-100%)*1.5*HR!$A$23/H9)))</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="F9" s="5">
+        <f>IF(P9&lt;=100%,HR!$B$1/I9, (100%*HR!$B$1/I9+((P9-100%)*1.5*HR!$B$1/I9)))</f>
+        <v>11.709693333333334</v>
+      </c>
+      <c r="G9" s="1">
         <v>0.3</v>
       </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9">
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>3</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>4</v>
       </c>
-      <c r="J9" s="5">
-        <f>(I9-H9)*$B$1</f>
+      <c r="K9" s="5">
+        <f>(J9-I9)*$B$1</f>
         <v>700</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>600</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="7">
-        <f>L9*$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="2">
-        <f>C9/H9*$B$3</f>
+      <c r="M9" s="1"/>
+      <c r="N9" s="7">
+        <f>M9*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <f>D9/I9*$B$3</f>
         <v>82.72</v>
       </c>
-      <c r="O9" s="10">
-        <f>$N$10/$P$5</f>
+      <c r="P9" s="10">
+        <f>$N$10/$Q$5</f>
         <v>1.16974</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>45</v>
       </c>
       <c r="N10" s="2">
-        <f>SUM(N5:N9)</f>
+        <f>SUM(O5:O9)</f>
         <v>701.84400000000005</v>
       </c>
       <c r="O10" s="12"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:18">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1469,7 +1493,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:18">
       <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
@@ -1489,7 +1513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="25.5">
+    <row r="14" spans="1:18" ht="25.5">
       <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
@@ -1509,7 +1533,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -1529,7 +1553,7 @@
         <v>13.62</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:18">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
@@ -1793,7 +1817,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1817,7 +1841,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1860,7 +1884,7 @@
   <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Check in Xlsx document
</commit_message>
<xml_diff>
--- a/Documents/BusinessSimulation.xlsx
+++ b/Documents/BusinessSimulation.xlsx
@@ -1178,8 +1178,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>